<commit_message>
Updated final group tracker progress.
</commit_message>
<xml_diff>
--- a/FinalProject/Submission/Group3FinalTodoList.xlsx
+++ b/FinalProject/Submission/Group3FinalTodoList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuan\OneDrive\Documents\Github\CSCI381-DataModeling-Group3\FinalProject\Submission\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\381DataModeling\Group3\CSCI381-DataModeling-Group3\FinalProject\Submission\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADBD77D-DBD7-4008-85BA-8066F8DE55E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EC0D33-708C-4987-A20D-57AE3682DDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34425" yWindow="1635" windowWidth="17280" windowHeight="12735" tabRatio="656" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ralph Granata" sheetId="1" r:id="rId1"/>
@@ -1439,7 +1439,7 @@
   <dimension ref="B1:H16"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1548,7 +1548,7 @@
     </row>
     <row r="9" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="12" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
@@ -1721,7 +1721,7 @@
   <dimension ref="B1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1874,7 +1874,7 @@
     </row>
     <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
@@ -1893,7 +1893,7 @@
     </row>
     <row r="12" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
@@ -2005,7 +2005,7 @@
   <dimension ref="B1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2114,7 +2114,7 @@
     </row>
     <row r="9" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -2156,7 +2156,7 @@
     </row>
     <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
@@ -2175,7 +2175,7 @@
     </row>
     <row r="12" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
@@ -2286,7 +2286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D7F7114-971E-49E2-8EA2-0E1816A122F1}">
   <dimension ref="B1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -2581,7 +2581,7 @@
   <dimension ref="B1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2690,7 +2690,7 @@
     </row>
     <row r="9" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -2732,7 +2732,7 @@
     </row>
     <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>31</v>
@@ -2751,7 +2751,7 @@
     </row>
     <row r="12" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
@@ -2862,8 +2862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2FA15D5-0168-4304-A7FC-CF44490ADCEB}">
   <dimension ref="B1:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2972,7 +2972,7 @@
     </row>
     <row r="9" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
@@ -3014,7 +3014,7 @@
     </row>
     <row r="11" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
@@ -3033,7 +3033,7 @@
     </row>
     <row r="12" spans="2:8" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>

</xml_diff>